<commit_message>
Changed PDF Generator to WS Request
</commit_message>
<xml_diff>
--- a/com.Goval.FacturaDigital/com.Goval.FacturaDigital.Android/Assets/FacturaGoval.xlsx
+++ b/com.Goval.FacturaDigital/com.Goval.FacturaDigital.Android/Assets/FacturaGoval.xlsx
@@ -18,6 +18,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$55</definedName>
     <definedName name="billDate">Sheet1!$J$3</definedName>
     <definedName name="billDescountAmount">Sheet1!$J$34</definedName>
+    <definedName name="billExpiration">Sheet1!$J$4</definedName>
     <definedName name="billId">Sheet1!$J$2</definedName>
     <definedName name="billTaxesAmount">Sheet1!$J$36</definedName>
     <definedName name="billTotal">Sheet1!$J$37</definedName>
@@ -387,14 +388,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <u/>
-      <sz val="22"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <u/>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -413,6 +406,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -750,79 +751,20 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -843,23 +785,82 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="26" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1232,8 +1233,8 @@
   </sheetPr>
   <dimension ref="A1:T441"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
@@ -1278,7 +1279,7 @@
       <c r="I2" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="107"/>
+      <c r="J2" s="113"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:20" ht="20.100000000000001" customHeight="1">
@@ -1296,16 +1297,16 @@
         <v>17</v>
       </c>
       <c r="J3" s="4"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="77"/>
-      <c r="S3" s="77"/>
-      <c r="T3" s="77"/>
+      <c r="K3" s="106"/>
+      <c r="L3" s="106"/>
+      <c r="M3" s="106"/>
+      <c r="N3" s="106"/>
+      <c r="O3" s="106"/>
+      <c r="P3" s="106"/>
+      <c r="Q3" s="106"/>
+      <c r="R3" s="106"/>
+      <c r="S3" s="106"/>
+      <c r="T3" s="106"/>
     </row>
     <row r="4" spans="1:20" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="31" t="s">
@@ -1437,17 +1438,17 @@
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1">
-      <c r="A12" s="103" t="s">
+      <c r="A12" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="105"/>
+      <c r="B12" s="86"/>
       <c r="C12" s="70"/>
-      <c r="D12" s="103" t="s">
+      <c r="D12" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="104"/>
-      <c r="F12" s="104"/>
-      <c r="G12" s="105"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="86"/>
       <c r="H12" s="34" t="s">
         <v>10</v>
       </c>
@@ -1460,15 +1461,15 @@
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:20" ht="15" customHeight="1">
-      <c r="A13" s="101"/>
-      <c r="B13" s="102"/>
+      <c r="A13" s="82"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="71"/>
-      <c r="D13" s="101" t="s">
+      <c r="D13" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="106"/>
-      <c r="F13" s="106"/>
-      <c r="G13" s="102"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="83"/>
       <c r="H13" s="32" t="s">
         <v>11</v>
       </c>
@@ -1477,24 +1478,24 @@
       </c>
       <c r="J13" s="72"/>
       <c r="K13" s="1"/>
-      <c r="M13" s="113"/>
+      <c r="M13" s="81"/>
     </row>
     <row r="14" spans="1:20" ht="15" customHeight="1">
-      <c r="A14" s="99"/>
-      <c r="B14" s="100"/>
+      <c r="A14" s="103"/>
+      <c r="B14" s="104"/>
       <c r="C14" s="15"/>
-      <c r="D14" s="83"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="85"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="101"/>
+      <c r="F14" s="101"/>
+      <c r="G14" s="102"/>
       <c r="H14" s="16"/>
       <c r="I14" s="33"/>
-      <c r="J14" s="110"/>
+      <c r="J14" s="78"/>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:20" ht="15" customHeight="1">
-      <c r="A15" s="81"/>
-      <c r="B15" s="82"/>
+      <c r="A15" s="98"/>
+      <c r="B15" s="99"/>
       <c r="C15" s="39"/>
       <c r="D15" s="27"/>
       <c r="E15" s="30"/>
@@ -1583,8 +1584,8 @@
       <c r="O20" s="18"/>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1">
-      <c r="A21" s="81"/>
-      <c r="B21" s="82"/>
+      <c r="A21" s="98"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="39"/>
       <c r="D21" s="27"/>
       <c r="E21" s="30"/>
@@ -1598,8 +1599,8 @@
       <c r="O21" s="17"/>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1">
-      <c r="A22" s="81"/>
-      <c r="B22" s="82"/>
+      <c r="A22" s="98"/>
+      <c r="B22" s="99"/>
       <c r="C22" s="39"/>
       <c r="D22" s="27"/>
       <c r="E22" s="30"/>
@@ -1628,8 +1629,8 @@
       <c r="O23" s="18"/>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1">
-      <c r="A24" s="81"/>
-      <c r="B24" s="82"/>
+      <c r="A24" s="98"/>
+      <c r="B24" s="99"/>
       <c r="C24" s="39"/>
       <c r="D24" s="27"/>
       <c r="E24" s="30"/>
@@ -1643,8 +1644,8 @@
       <c r="O24" s="18"/>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1">
-      <c r="A25" s="81"/>
-      <c r="B25" s="82"/>
+      <c r="A25" s="98"/>
+      <c r="B25" s="99"/>
       <c r="C25" s="39"/>
       <c r="D25" s="27"/>
       <c r="E25" s="30"/>
@@ -1658,14 +1659,14 @@
       <c r="O25" s="17"/>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1">
-      <c r="A26" s="81"/>
-      <c r="B26" s="82"/>
+      <c r="A26" s="98"/>
+      <c r="B26" s="99"/>
       <c r="C26" s="39"/>
       <c r="D26" s="27"/>
       <c r="E26" s="30"/>
       <c r="F26" s="30"/>
       <c r="G26" s="13"/>
-      <c r="H26" s="109"/>
+      <c r="H26" s="77"/>
       <c r="I26" s="33"/>
       <c r="J26" s="33"/>
       <c r="K26" s="1"/>
@@ -1703,44 +1704,44 @@
       <c r="O28" s="18"/>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1">
-      <c r="A29" s="91"/>
-      <c r="B29" s="92"/>
+      <c r="A29" s="96"/>
+      <c r="B29" s="97"/>
       <c r="C29" s="39"/>
-      <c r="D29" s="78" t="s">
+      <c r="D29" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="E29" s="79"/>
-      <c r="F29" s="79"/>
-      <c r="G29" s="80"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="95"/>
       <c r="H29" s="73"/>
       <c r="I29" s="33"/>
-      <c r="J29" s="111"/>
+      <c r="J29" s="79"/>
       <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1">
-      <c r="A30" s="91"/>
-      <c r="B30" s="92"/>
+      <c r="A30" s="96"/>
+      <c r="B30" s="97"/>
       <c r="C30" s="39"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="79"/>
-      <c r="G30" s="80"/>
+      <c r="D30" s="93"/>
+      <c r="E30" s="94"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="95"/>
       <c r="H30" s="73"/>
       <c r="I30" s="33"/>
-      <c r="J30" s="111"/>
+      <c r="J30" s="79"/>
       <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:15" ht="15" customHeight="1">
-      <c r="A31" s="86"/>
-      <c r="B31" s="87"/>
+      <c r="A31" s="88"/>
+      <c r="B31" s="89"/>
       <c r="C31" s="74"/>
-      <c r="D31" s="88"/>
-      <c r="E31" s="89"/>
-      <c r="F31" s="89"/>
-      <c r="G31" s="90"/>
+      <c r="D31" s="90"/>
+      <c r="E31" s="91"/>
+      <c r="F31" s="91"/>
+      <c r="G31" s="92"/>
       <c r="H31" s="75"/>
       <c r="I31" s="42"/>
-      <c r="J31" s="112"/>
+      <c r="J31" s="80"/>
       <c r="K31" s="1"/>
     </row>
     <row r="32" spans="1:15" ht="13.8">
@@ -1764,10 +1765,10 @@
       <c r="E33" s="43"/>
       <c r="F33" s="43"/>
       <c r="G33" s="43"/>
-      <c r="H33" s="93" t="s">
+      <c r="H33" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="I33" s="94"/>
+      <c r="I33" s="108"/>
       <c r="J33" s="51"/>
       <c r="K33" s="1"/>
       <c r="N33" s="21"/>
@@ -1781,10 +1782,10 @@
       <c r="E34" s="43"/>
       <c r="F34" s="43"/>
       <c r="G34" s="43"/>
-      <c r="H34" s="97" t="s">
+      <c r="H34" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="I34" s="98"/>
+      <c r="I34" s="112"/>
       <c r="J34" s="52"/>
       <c r="K34" s="1"/>
       <c r="N34" s="21"/>
@@ -1800,27 +1801,27 @@
       <c r="E35" s="54"/>
       <c r="F35" s="54"/>
       <c r="G35" s="43"/>
-      <c r="H35" s="97" t="s">
+      <c r="H35" s="111" t="s">
         <v>3</v>
       </c>
-      <c r="I35" s="98"/>
+      <c r="I35" s="112"/>
       <c r="J35" s="52"/>
       <c r="K35" s="1"/>
       <c r="N35" s="21"/>
       <c r="O35" s="20"/>
     </row>
     <row r="36" spans="1:15" ht="19.2" customHeight="1">
-      <c r="A36" s="108"/>
+      <c r="A36" s="76"/>
       <c r="B36" s="55"/>
       <c r="C36" s="55"/>
       <c r="D36" s="55"/>
       <c r="E36" s="55"/>
       <c r="F36" s="55"/>
       <c r="G36" s="43"/>
-      <c r="H36" s="97" t="s">
+      <c r="H36" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="I36" s="98"/>
+      <c r="I36" s="112"/>
       <c r="J36" s="52"/>
       <c r="K36" s="1"/>
       <c r="N36" s="21"/>
@@ -1834,10 +1835,10 @@
       <c r="E37" s="54"/>
       <c r="F37" s="54"/>
       <c r="G37" s="43"/>
-      <c r="H37" s="95" t="s">
+      <c r="H37" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="I37" s="96"/>
+      <c r="I37" s="110"/>
       <c r="J37" s="53"/>
       <c r="K37" s="1"/>
       <c r="N37" s="21"/>
@@ -1979,10 +1980,10 @@
       </c>
       <c r="B46" s="60"/>
       <c r="C46" s="60"/>
-      <c r="D46" s="76" t="s">
+      <c r="D46" s="105" t="s">
         <v>35</v>
       </c>
-      <c r="E46" s="76"/>
+      <c r="E46" s="105"/>
       <c r="F46" s="61" t="s">
         <v>37</v>
       </c>
@@ -2000,10 +2001,10 @@
       </c>
       <c r="B47" s="60"/>
       <c r="C47" s="60"/>
-      <c r="D47" s="76" t="s">
+      <c r="D47" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="E47" s="76"/>
+      <c r="E47" s="105"/>
       <c r="F47" s="61" t="s">
         <v>37</v>
       </c>
@@ -2021,10 +2022,10 @@
       </c>
       <c r="B48" s="60"/>
       <c r="C48" s="60"/>
-      <c r="D48" s="76" t="s">
+      <c r="D48" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="E48" s="76"/>
+      <c r="E48" s="105"/>
       <c r="F48" s="61" t="s">
         <v>37</v>
       </c>
@@ -8314,6 +8315,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="K3:T3"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H34:I34"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="D12:G12"/>
     <mergeCell ref="D13:G13"/>
@@ -8330,17 +8342,6 @@
     <mergeCell ref="D14:G14"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="K3:T3"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H34:I34"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>